<commit_message>
Domino Single USB tile Revision B
</commit_message>
<xml_diff>
--- a/Domino Single USB/BOM/Domino Single USB BOM.xlsx
+++ b/Domino Single USB/BOM/Domino Single USB BOM.xlsx
@@ -8,29 +8,30 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Single USB Rev. A" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Single USB Rev. B" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single USB Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single USB Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single USB Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. A'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Item</t>
   </si>
@@ -107,10 +108,10 @@
     <t>CAP CER 0.1UF 50V 10% X7R 0402</t>
   </si>
   <si>
-    <t>YSSR05</t>
-  </si>
-  <si>
-    <t>YEASHIN</t>
+    <t>PRTR5V0U2X</t>
+  </si>
+  <si>
+    <t>NXP</t>
   </si>
   <si>
     <t>SOT143B</t>
@@ -140,16 +141,28 @@
     <t>PTC RESETTBLE 1.10A 8V CHIP 1812</t>
   </si>
   <si>
-    <t>MH4-1</t>
-  </si>
-  <si>
-    <t>MH4-1-0.1</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT .100 1ROW 4POS 8.08 HEAD 3.05 TAIL 15AU</t>
+    <t>MH10-1</t>
+  </si>
+  <si>
+    <t>MH10-1-0.1</t>
+  </si>
+  <si>
+    <t>J1, J3</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT .100 1ROW 10POS 8.08 HEAD 3.05 TAIL 15AU</t>
+  </si>
+  <si>
+    <t>USB_AF-006</t>
+  </si>
+  <si>
+    <t>SZJUSTWELL ELECTRONICS</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>CONN USB A RECPT SMT R/A VERT</t>
   </si>
   <si>
     <t>BLM31PG601SN1L</t>
@@ -167,16 +180,19 @@
     <t>FERRITE CHIP 600 OHM 1500MA 1206</t>
   </si>
   <si>
-    <t>USB_AF-020</t>
-  </si>
-  <si>
-    <t>SZJUSTWELL ELECTRONICS</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>CONN USB A RECPT T/H R/A VERT</t>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>R0402_0R_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>R5, R6</t>
+  </si>
+  <si>
+    <t>RES 0.0 OHM 1/16W JUMP 0402 SMD</t>
   </si>
 </sst>
 </file>
@@ -287,22 +303,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E7" activeCellId="0" pane="topLeft" sqref="E7"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2:H10"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.7921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.9843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8039215686274"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.8588235294118"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.9843137254902"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.7607843137255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.356862745098"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3019607843137"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.81176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.1098039215686"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9450980392157"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.0117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.1098039215686"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.956862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.6627450980392"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -469,7 +485,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>36</v>
@@ -507,13 +523,13 @@
         <v>40</v>
       </c>
       <c r="F8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="H8" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
@@ -524,22 +540,48 @@
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="E9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>47</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Domino Single USB Rev. C: changed Logos
</commit_message>
<xml_diff>
--- a/Domino Single USB/BOM/Domino Single USB BOM.xlsx
+++ b/Domino Single USB/BOM/Domino Single USB BOM.xlsx
@@ -8,23 +8,24 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Single USB Rev. B" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Single USB Rev. C" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -306,19 +307,19 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2:H10"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.81176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.1098039215686"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9450980392157"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.0117647058824"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.1098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.956862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.6627450980392"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.72941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.83921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.2470588235294"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0823529411765"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.1686274509804"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.2470588235294"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.156862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.9725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.77254901960784"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
Domino Single USB Rev. C: removed the resetable fuse that causes too much drop for high-current USB devices
</commit_message>
<xml_diff>
--- a/Domino Single USB/BOM/Domino Single USB BOM.xlsx
+++ b/Domino Single USB/BOM/Domino Single USB BOM.xlsx
@@ -11,28 +11,29 @@
     <sheet name="Domino Single USB Rev. C" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$10</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>Item</t>
   </si>
@@ -122,24 +123,6 @@
   </si>
   <si>
     <t>TVS DIODE ARRAY 2CH 5V SOT143</t>
-  </si>
-  <si>
-    <t>0ZCA0050FF2G</t>
-  </si>
-  <si>
-    <t>BEL FUSE INC</t>
-  </si>
-  <si>
-    <t>0ZCG0110FF2C</t>
-  </si>
-  <si>
-    <t>PTC1206</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>PTC RESETTBLE 1.10A 8V CHIP 1812</t>
   </si>
   <si>
     <t>MH10-1</t>
@@ -304,22 +287,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+      <selection activeCell="A9" activeCellId="0" pane="topLeft" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.83921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.2470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.1686274509804"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.2470588235294"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.156862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.9725490196078"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5372549019608"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3725490196078"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2196078431373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.321568627451"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3725490196078"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.356862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.278431372549"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.6549019607843"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81960784313726"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -460,25 +443,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
@@ -486,25 +469,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="H7" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
@@ -515,22 +498,22 @@
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>40</v>
       </c>
       <c r="G8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
@@ -538,51 +521,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>44</v>
       </c>
       <c r="F9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="A10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added USB power switch to Sinfle USB tile
</commit_message>
<xml_diff>
--- a/Domino Single USB/BOM/Domino Single USB BOM.xlsx
+++ b/Domino Single USB/BOM/Domino Single USB BOM.xlsx
@@ -8,32 +8,33 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Single USB Rev. C" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Single USB Rev. D" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
   <si>
     <t>Item</t>
   </si>
@@ -62,54 +63,81 @@
     <t>Remarks</t>
   </si>
   <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>ANY</t>
+  </si>
+  <si>
+    <t>C0603_10u_X5R_20%_CER_6V3</t>
+  </si>
+  <si>
+    <t>C0603</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 6.3V 20% X5R 0603</t>
+  </si>
+  <si>
+    <t>220u</t>
+  </si>
+  <si>
+    <t>CPOLC-6032_220u_20%_TANT_10V</t>
+  </si>
+  <si>
+    <t>C/6032-25</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>CAP TANT 220UF 10V 20% 2413</t>
+  </si>
+  <si>
+    <t>100n</t>
+  </si>
+  <si>
+    <t>C0402_100n_X7R_10%_CER_50V</t>
+  </si>
+  <si>
+    <t>C0402</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V 10% X7R 0402</t>
+  </si>
+  <si>
+    <t>C0805_10u_X5R_10%_CER_16V</t>
+  </si>
+  <si>
+    <t>C0805</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 16V 10% X5R 0805</t>
+  </si>
+  <si>
     <t>1n</t>
   </si>
   <si>
-    <t>ANY</t>
-  </si>
-  <si>
     <t>C1206_1n_X7R_10%_CER_500V</t>
   </si>
   <si>
     <t>C1206</t>
   </si>
   <si>
-    <t>C1</t>
+    <t>C5</t>
   </si>
   <si>
     <t>CAP CER 1000PF 500V 10% X7R 1206</t>
   </si>
   <si>
-    <t>10u</t>
-  </si>
-  <si>
-    <t>C0805_10u_X5R_10%_CER_16V</t>
-  </si>
-  <si>
-    <t>C0805</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>CAP CER 10UF 16V 10% X5R 0805</t>
-  </si>
-  <si>
-    <t>100n</t>
-  </si>
-  <si>
-    <t>C0402_100n_X7R_10%_CER_50V</t>
-  </si>
-  <si>
-    <t>C0402</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 50V 10% X7R 0402</t>
-  </si>
-  <si>
     <t>PRTR5V0U2X</t>
   </si>
   <si>
@@ -131,7 +159,7 @@
     <t>MH10-1-0.1</t>
   </si>
   <si>
-    <t>J1, J3</t>
+    <t>J1, J2</t>
   </si>
   <si>
     <t>CONN HEADER VERT .100 1ROW 10POS 8.08 HEAD 3.05 TAIL 15AU</t>
@@ -143,7 +171,7 @@
     <t>SZJUSTWELL ELECTRONICS</t>
   </si>
   <si>
-    <t>J2</t>
+    <t>J3</t>
   </si>
   <si>
     <t>CONN USB A RECPT SMT R/A VERT</t>
@@ -164,19 +192,58 @@
     <t>FERRITE CHIP 600 OHM 1500MA 1206</t>
   </si>
   <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>R0402_100k_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>RES 100K OHM 1/16W 5% 0402 SMD</t>
+  </si>
+  <si>
+    <t>15k</t>
+  </si>
+  <si>
+    <t>R0402_15k_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RES 15K OHM 1/16W 5% 0402 SMD</t>
+  </si>
+  <si>
     <t>0R</t>
   </si>
   <si>
     <t>R0402_0R_5%_62.5mW</t>
   </si>
   <si>
-    <t>R0402</t>
-  </si>
-  <si>
-    <t>R5, R6</t>
+    <t>R3, R4</t>
   </si>
   <si>
     <t>RES 0.0 OHM 1/16W JUMP 0402 SMD</t>
+  </si>
+  <si>
+    <t>MP65151DJ</t>
+  </si>
+  <si>
+    <t>MONOLITHIC POWER</t>
+  </si>
+  <si>
+    <t>SOT23-6</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>IC POWER SWITCH 1.7A SOT23-6</t>
   </si>
 </sst>
 </file>
@@ -287,22 +354,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A9" activeCellId="0" pane="topLeft" sqref="A9"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2196078431373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.321568627451"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3725490196078"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.356862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.278431372549"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.6549019607843"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.88235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4980392156863"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.3647058823529"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.4745098039216"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.4980392156863"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.5960784313726"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.86274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -420,22 +487,22 @@
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
@@ -443,16 +510,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>31</v>
@@ -481,13 +548,13 @@
         <v>34</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
@@ -495,16 +562,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>40</v>
@@ -521,25 +588,155 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>43</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>47</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Domino Single USB tile Rev. D: added resistors en power siwtch feedback and enable, changed output capacitor to smaller one
</commit_message>
<xml_diff>
--- a/Domino Single USB/BOM/Domino Single USB BOM.xlsx
+++ b/Domino Single USB/BOM/Domino Single USB BOM.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Domino Single USB Rev. D" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$15</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
@@ -22,19 +22,20 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
   <si>
     <t>Item</t>
   </si>
@@ -63,12 +64,42 @@
     <t>Remarks</t>
   </si>
   <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>ANY</t>
+  </si>
+  <si>
+    <t>R0402_0R_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>R3, R5, R6</t>
+  </si>
+  <si>
+    <t>RES 0.0 OHM 1/16W JUMP 0402 SMD</t>
+  </si>
+  <si>
+    <t>1n</t>
+  </si>
+  <si>
+    <t>C1206_1n_X7R_10%_CER_500V</t>
+  </si>
+  <si>
+    <t>C1206</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 500V 10% X7R 1206</t>
+  </si>
+  <si>
     <t>10u</t>
   </si>
   <si>
-    <t>ANY</t>
-  </si>
-  <si>
     <t>C0603_10u_X5R_20%_CER_6V3</t>
   </si>
   <si>
@@ -81,19 +112,64 @@
     <t>CAP CER 10UF 6.3V 20% X5R 0603</t>
   </si>
   <si>
-    <t>220u</t>
-  </si>
-  <si>
-    <t>CPOLC-6032_220u_20%_TANT_10V</t>
-  </si>
-  <si>
-    <t>C/6032-25</t>
+    <t>C0805_10u_X5R_10%_CER_16V</t>
+  </si>
+  <si>
+    <t>C0805</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 16V 10% X5R 0805</t>
+  </si>
+  <si>
+    <t>15k</t>
+  </si>
+  <si>
+    <t>R0402_15k_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>RES 15K OHM 1/16W 5% 0402 SMD</t>
+  </si>
+  <si>
+    <t>22u</t>
+  </si>
+  <si>
+    <t>C0805_22u_X5R_20%_CER_6V3</t>
   </si>
   <si>
     <t>C2</t>
   </si>
   <si>
-    <t>CAP TANT 220UF 10V 20% 2413</t>
+    <t>CAP CER 22UF 6.3V 20% X5R 0805</t>
+  </si>
+  <si>
+    <t>33R</t>
+  </si>
+  <si>
+    <t>R0402_33R_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>RES 33 OHM 1/16W 5% 0402 SMD</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>R0402_100k_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RES 100K OHM 1/16W 5% 0402 SMD</t>
   </si>
   <si>
     <t>100n</t>
@@ -111,31 +187,46 @@
     <t>CAP CER 0.1UF 50V 10% X7R 0402</t>
   </si>
   <si>
-    <t>C0805_10u_X5R_10%_CER_16V</t>
-  </si>
-  <si>
-    <t>C0805</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>CAP CER 10UF 16V 10% X5R 0805</t>
-  </si>
-  <si>
-    <t>1n</t>
-  </si>
-  <si>
-    <t>C1206_1n_X7R_10%_CER_500V</t>
-  </si>
-  <si>
-    <t>C1206</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>CAP CER 1000PF 500V 10% X7R 1206</t>
+    <t>BLM31PG601SN1L</t>
+  </si>
+  <si>
+    <t>MURATA</t>
+  </si>
+  <si>
+    <t>FB1206</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>FERRITE CHIP 600 OHM 1500MA 1206</t>
+  </si>
+  <si>
+    <t>MH10-1</t>
+  </si>
+  <si>
+    <t>MH10-1-0.1</t>
+  </si>
+  <si>
+    <t>J1, J2</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT .100 1ROW 10POS 8.08 HEAD 3.05 TAIL 15AU</t>
+  </si>
+  <si>
+    <t>MP65151DJ</t>
+  </si>
+  <si>
+    <t>MONOLITHIC POWER</t>
+  </si>
+  <si>
+    <t>SOT23-6</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>IC POWER SWITCH 1.7A SOT23-6</t>
   </si>
   <si>
     <t>PRTR5V0U2X</t>
@@ -153,18 +244,6 @@
     <t>TVS DIODE ARRAY 2CH 5V SOT143</t>
   </si>
   <si>
-    <t>MH10-1</t>
-  </si>
-  <si>
-    <t>MH10-1-0.1</t>
-  </si>
-  <si>
-    <t>J1, J2</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT .100 1ROW 10POS 8.08 HEAD 3.05 TAIL 15AU</t>
-  </si>
-  <si>
     <t>USB_AF-006</t>
   </si>
   <si>
@@ -175,75 +254,6 @@
   </si>
   <si>
     <t>CONN USB A RECPT SMT R/A VERT</t>
-  </si>
-  <si>
-    <t>BLM31PG601SN1L</t>
-  </si>
-  <si>
-    <t>MURATA</t>
-  </si>
-  <si>
-    <t>FB1206</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>FERRITE CHIP 600 OHM 1500MA 1206</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>R0402_100k_5%_62.5mW</t>
-  </si>
-  <si>
-    <t>R0402</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>RES 100K OHM 1/16W 5% 0402 SMD</t>
-  </si>
-  <si>
-    <t>15k</t>
-  </si>
-  <si>
-    <t>R0402_15k_5%_62.5mW</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>RES 15K OHM 1/16W 5% 0402 SMD</t>
-  </si>
-  <si>
-    <t>0R</t>
-  </si>
-  <si>
-    <t>R0402_0R_5%_62.5mW</t>
-  </si>
-  <si>
-    <t>R3, R4</t>
-  </si>
-  <si>
-    <t>RES 0.0 OHM 1/16W JUMP 0402 SMD</t>
-  </si>
-  <si>
-    <t>MP65151DJ</t>
-  </si>
-  <si>
-    <t>MONOLITHIC POWER</t>
-  </si>
-  <si>
-    <t>SOT23-6</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>IC POWER SWITCH 1.7A SOT23-6</t>
   </si>
 </sst>
 </file>
@@ -354,22 +364,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.88235294117647"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4980392156863"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.3647058823529"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.4745098039216"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.4980392156863"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.5960784313726"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.90980392156863"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.6352941176471"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5058823529412"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.6274509803922"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.6352941176471"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.7529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.9137254901961"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.8901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.90980392156863"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -406,7 +416,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>9</v>
@@ -487,7 +497,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>10</v>
@@ -522,13 +532,13 @@
         <v>30</v>
       </c>
       <c r="F6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
@@ -539,22 +549,22 @@
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>34</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>38</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
@@ -562,25 +572,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="H8" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
@@ -591,25 +601,25 @@
         <v>1</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
@@ -617,103 +627,103 @@
         <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="G10" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="0" t="s">
+      <c r="H10" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
-      <c r="A11" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="E11" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="G11" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="H11" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="G13" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="0" t="s">
+      <c r="H13" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
@@ -721,22 +731,48 @@
         <v>1</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="E14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>69</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Domino Single USB Rev. E: changed silkscreen font ratio to 20%
</commit_message>
<xml_diff>
--- a/Domino Single USB/BOM/Domino Single USB BOM.xlsx
+++ b/Domino Single USB/BOM/Domino Single USB BOM.xlsx
@@ -8,27 +8,28 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Single USB Rev. D" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Single USB Rev. E" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Single USB Rev. E'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -371,15 +372,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.90980392156863"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.6352941176471"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5058823529412"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.6274509803922"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.6352941176471"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.7529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.9137254901961"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.8901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.90980392156863"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.92941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7725490196078"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.643137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.7803921568627"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7725490196078"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.9607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2274509803922"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.0078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.95294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -749,7 +750,7 @@
         <v>68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>

</xml_diff>